<commit_message>
added web service added some tabels for valdiation CN5
</commit_message>
<xml_diff>
--- a/Tabellen/Objekte im Bad.xlsx
+++ b/Tabellen/Objekte im Bad.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="47">
   <si>
     <t xml:space="preserve">Toilette</t>
   </si>
@@ -103,6 +103,9 @@
     <t xml:space="preserve">695432503_df40a4c789.jpg</t>
   </si>
   <si>
+    <t xml:space="preserve">Summe</t>
+  </si>
+  <si>
     <t xml:space="preserve">Conceptnet Relatedness</t>
   </si>
   <si>
@@ -143,6 +146,21 @@
   </si>
   <si>
     <t xml:space="preserve">towels</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rangfolge</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bad</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Klopapier</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zahnbürste</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Zahnpasta</t>
   </si>
 </sst>
 </file>
@@ -270,10 +288,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:R16"/>
+  <dimension ref="A1:T48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="I1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="M17" activeCellId="0" sqref="M17"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F23" activeCellId="0" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -391,6 +409,9 @@
       <c r="R2" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="T2" s="1" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="2" t="s">
@@ -447,6 +468,9 @@
       <c r="R3" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="T3" s="1" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="2" t="s">
@@ -503,6 +527,9 @@
       <c r="R4" s="2" t="n">
         <v>1</v>
       </c>
+      <c r="T4" s="1" t="s">
+        <v>11</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="s">
@@ -559,6 +586,9 @@
       <c r="R5" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="T5" s="2" t="s">
+        <v>1</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="s">
@@ -615,6 +645,9 @@
       <c r="R6" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="T6" s="1" t="s">
+        <v>10</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
@@ -671,6 +704,9 @@
       <c r="R7" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="T7" s="1" t="s">
+        <v>2</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="2" t="s">
@@ -727,6 +763,9 @@
       <c r="R8" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="T8" s="1" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="2" t="s">
@@ -783,6 +822,9 @@
       <c r="R9" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="T9" s="1" t="s">
+        <v>4</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
@@ -839,6 +881,9 @@
       <c r="R10" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="T10" s="1" t="s">
+        <v>0</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="s">
@@ -895,8 +940,14 @@
       <c r="R11" s="2" t="n">
         <v>0</v>
       </c>
+      <c r="T11" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="s">
+        <v>27</v>
+      </c>
       <c r="B12" s="0" t="n">
         <f aca="false">SUM(#REF!)</f>
         <v>8</v>
@@ -968,7 +1019,7 @@
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>0.8</v>
@@ -1012,40 +1063,40 @@
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B14" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="J14" s="0" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="K14" s="0" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="L14" s="0" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="M14" s="0" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="P14" s="0" t="s">
         <v>14</v>
@@ -1058,7 +1109,177 @@
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="M16" s="0" t="s">
-        <v>40</v>
+        <v>41</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="s">
+        <v>42</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="E17" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="F17" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="H17" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="I17" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="L17" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="M17" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="P17" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A39" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A41" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B42" s="0" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A43" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B43" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B44" s="0" t="n">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A45" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B46" s="0" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A47" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B47" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B48" s="0" t="n">
+        <v>10</v>
       </c>
     </row>
   </sheetData>

</xml_diff>